<commit_message>
feat(network): adiciona inicio, finalização, vitoria e inicio dos ataques
</commit_message>
<xml_diff>
--- a/comandos.xlsx
+++ b/comandos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Descrição</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Direcional</t>
   </si>
   <si>
+    <t>A finalizar</t>
+  </si>
+  <si>
     <t>Ataque Morte dos Promogênitos</t>
   </si>
   <si>
@@ -106,7 +109,7 @@
     <t>VITORIA</t>
   </si>
   <si>
-    <t>VITORIA#&lt;ID&gt;</t>
+    <t>VITORIA#&lt;NOME&gt;</t>
   </si>
   <si>
     <t>Iniciar Jogo</t>
@@ -135,10 +138,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -159,15 +162,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,29 +176,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,16 +190,93 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,7 +291,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,53 +299,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,37 +313,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,145 +493,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,15 +504,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -528,24 +522,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -557,21 +533,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,6 +554,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -601,162 +571,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.2" outlineLevelCol="5"/>
@@ -1104,16 +1104,16 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1127,17 +1127,17 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1147,61 +1147,70 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
+      <c r="F5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
@@ -1210,18 +1219,18 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
@@ -1230,90 +1239,102 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>27</v>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>33</v>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>33</v>
+      <c r="E12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>